<commit_message>
Update PMOInformatica Plantilla de Product Backlog (4) (version 1).xlsx
</commit_message>
<xml_diff>
--- a/CRIALED/DOCUMENTOS/PMOInformatica Plantilla de Product Backlog (4) (version 1).xlsx
+++ b/CRIALED/DOCUMENTOS/PMOInformatica Plantilla de Product Backlog (4) (version 1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Downloads\PMO BACK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Documents\GitHub\CRIALED---APLICACIONES-INFORM-TICAS-II\CRIALED---APLICACIONES-INFORM-TICAS-II\CRIALED\DOCUMENTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDA453CC-C5E5-4B60-8079-4F0225F838BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF979B5C-908F-48C2-B638-0B842C865AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="102">
   <si>
     <t>Columna</t>
   </si>
@@ -350,6 +349,9 @@
   </si>
   <si>
     <t>Sprint 7</t>
+  </si>
+  <si>
+    <t>dfdfdfd</t>
   </si>
 </sst>
 </file>
@@ -841,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="48" zoomScaleNormal="48" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="48" zoomScaleNormal="48" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1179,9 @@
       <c r="I10" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="M10" s="14"/>
+      <c r="M10" s="14" t="s">
+        <v>101</v>
+      </c>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>

</xml_diff>